<commit_message>
Service and 2nd dataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{F6A6C4C9-8BC0-4808-BEC7-FAD91032B517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{64B56FE4-4DFD-46A5-B364-53F682198174}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BFB3AA1E-22B9-4E35-96F4-21EFF30EAC82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9015" yWindow="4830" windowWidth="19170" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="29070" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmarks" sheetId="1" r:id="rId1"/>
+    <sheet name="2ndTest" sheetId="3" r:id="rId2"/>
+    <sheet name="others" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Execute</t>
   </si>
@@ -69,6 +72,15 @@
   </si>
   <si>
     <t>amd4</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>ryzen 7</t>
+  </si>
+  <si>
+    <t>r1</t>
   </si>
 </sst>
 </file>
@@ -512,26 +524,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -539,22 +552,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="3"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -562,100 +578,256 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>95</v>
       </c>
-      <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="6">
-        <v>149</v>
-      </c>
-      <c r="G3" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="6">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="6">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12" s="2"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1048576" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375DB3CA-EB16-47D9-B257-1E8C47EF936A}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E3143D-60F4-4A70-A1EF-CF417FF3D1CD}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="A2:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>